<commit_message>
adding data upto october 2025
</commit_message>
<xml_diff>
--- a/data/Lakshadweep.xlsx
+++ b/data/Lakshadweep.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Vehicle Category Month Wise Data  of Lakshadweep (2025)</t>
   </si>
@@ -56,19 +56,31 @@
     <t>AUG</t>
   </si>
   <si>
+    <t>SEP</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>NOV</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>THREE WHEELER(T)</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>TWO WHEELER(NT)</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -143,14 +155,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="2.2109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="18.88671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="19.2265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="4.2109375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="4.515625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.15234375" customWidth="true" bestFit="true"/>
@@ -159,7 +171,10 @@
     <col min="8" max="8" width="4.296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="3.94921875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="5.0625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="2.2109375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="4.47265625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="4.88671875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="5.11328125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="2.2109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -177,7 +192,7 @@
       <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="K2" t="s" s="5">
+      <c r="N2" t="s" s="5">
         <v>4</v>
       </c>
     </row>
@@ -216,52 +231,114 @@
         <v>13</v>
       </c>
       <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10"/>
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <printOptions gridLines="true"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>